<commit_message>
Amend data to include ID column
</commit_message>
<xml_diff>
--- a/ELISA_data/091918 IL10 Plate 1.xlsx
+++ b/ELISA_data/091918 IL10 Plate 1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28705"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="72">
   <si>
     <t>Software Version</t>
   </si>
@@ -238,6 +238,9 @@
   </si>
   <si>
     <t>B12.b, 2FL, HK</t>
+  </si>
+  <si>
+    <t>ID</t>
   </si>
 </sst>
 </file>
@@ -404,8 +407,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="55">
+  <cellStyleXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -520,7 +525,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="55">
+  <cellStyles count="57">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -548,6 +553,7 @@
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -575,6 +581,7 @@
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -845,7 +852,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1398,7 +1405,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
@@ -1789,15 +1796,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E61"/>
+  <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>40</v>
       </c>
@@ -1813,8 +1820,11 @@
       <c r="E1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="9">
         <v>0.32700000000000001</v>
       </c>
@@ -1830,8 +1840,11 @@
       <c r="E2">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="15">
         <v>0.39900000000000002</v>
       </c>
@@ -1847,8 +1860,11 @@
       <c r="E3">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="14">
         <v>0.64300000000000002</v>
       </c>
@@ -1864,8 +1880,11 @@
       <c r="E4">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="15">
         <v>0.376</v>
       </c>
@@ -1881,8 +1900,11 @@
       <c r="E5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="8">
         <v>0.51400000000000001</v>
       </c>
@@ -1898,8 +1920,11 @@
       <c r="E6">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="F6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="15">
         <v>0.376</v>
       </c>
@@ -1915,8 +1940,11 @@
       <c r="E7">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="F7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="10">
         <v>0.17799999999999999</v>
       </c>
@@ -1932,8 +1960,11 @@
       <c r="E8">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="F8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="11">
         <v>0.11700000000000001</v>
       </c>
@@ -1949,8 +1980,11 @@
       <c r="E9">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="F9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="16">
         <v>0.26400000000000001</v>
       </c>
@@ -1966,8 +2000,11 @@
       <c r="E10">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="F10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="12">
         <v>7.5999999999999998E-2</v>
       </c>
@@ -1983,8 +2020,11 @@
       <c r="E11">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="F11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="10">
         <v>0.18</v>
       </c>
@@ -2000,8 +2040,11 @@
       <c r="E12">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="F12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" s="16">
         <v>0.28599999999999998</v>
       </c>
@@ -2017,8 +2060,11 @@
       <c r="E13">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="F13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" s="10">
         <v>0.23300000000000001</v>
       </c>
@@ -2034,8 +2080,11 @@
       <c r="E14">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="F14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" s="10">
         <v>0.23899999999999999</v>
       </c>
@@ -2051,8 +2100,11 @@
       <c r="E15">
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="F15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" s="8">
         <v>0.54600000000000004</v>
       </c>
@@ -2068,8 +2120,11 @@
       <c r="E16">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="F16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" s="17">
         <v>0.68899999999999995</v>
       </c>
@@ -2085,8 +2140,11 @@
       <c r="E17">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="F17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" s="8">
         <v>0.52400000000000002</v>
       </c>
@@ -2102,8 +2160,11 @@
       <c r="E18">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="F18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" s="18">
         <v>0.85599999999999998</v>
       </c>
@@ -2119,8 +2180,11 @@
       <c r="E19">
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="F19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" s="14">
         <v>0.628</v>
       </c>
@@ -2136,8 +2200,11 @@
       <c r="E20">
         <v>4</v>
       </c>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="F20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" s="19">
         <v>0.48499999999999999</v>
       </c>
@@ -2153,8 +2220,11 @@
       <c r="E21">
         <v>4</v>
       </c>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="F21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" s="15">
         <v>0.371</v>
       </c>
@@ -2170,8 +2240,11 @@
       <c r="E22">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="F22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" s="19">
         <v>0.45</v>
       </c>
@@ -2187,8 +2260,11 @@
       <c r="E23">
         <v>4</v>
       </c>
-    </row>
-    <row r="24" spans="1:5">
+      <c r="F23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" s="15">
         <v>0.40200000000000002</v>
       </c>
@@ -2204,8 +2280,11 @@
       <c r="E24">
         <v>4</v>
       </c>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="F24">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" s="19">
         <v>0.45300000000000001</v>
       </c>
@@ -2221,8 +2300,11 @@
       <c r="E25">
         <v>4</v>
       </c>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="F25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" s="17">
         <v>0.70399999999999996</v>
       </c>
@@ -2238,8 +2320,11 @@
       <c r="E26">
         <v>4</v>
       </c>
-    </row>
-    <row r="27" spans="1:5">
+      <c r="F26">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" s="20">
         <v>0.58399999999999996</v>
       </c>
@@ -2255,8 +2340,11 @@
       <c r="E27">
         <v>4</v>
       </c>
-    </row>
-    <row r="28" spans="1:5">
+      <c r="F27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" s="8">
         <v>0.55200000000000005</v>
       </c>
@@ -2272,8 +2360,11 @@
       <c r="E28">
         <v>4</v>
       </c>
-    </row>
-    <row r="29" spans="1:5">
+      <c r="F28">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29" s="15">
         <v>0.38500000000000001</v>
       </c>
@@ -2289,8 +2380,11 @@
       <c r="E29">
         <v>4</v>
       </c>
-    </row>
-    <row r="30" spans="1:5">
+      <c r="F29">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30" s="20">
         <v>0.61099999999999999</v>
       </c>
@@ -2306,8 +2400,11 @@
       <c r="E30">
         <v>4</v>
       </c>
-    </row>
-    <row r="31" spans="1:5">
+      <c r="F30">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31" s="15">
         <v>0.38</v>
       </c>
@@ -2323,8 +2420,11 @@
       <c r="E31">
         <v>4</v>
       </c>
-    </row>
-    <row r="32" spans="1:5">
+      <c r="F31">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32" s="16">
         <v>0.25</v>
       </c>
@@ -2340,8 +2440,11 @@
       <c r="E32">
         <v>4</v>
       </c>
-    </row>
-    <row r="33" spans="1:5">
+      <c r="F32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33" s="9">
         <v>0.35099999999999998</v>
       </c>
@@ -2357,8 +2460,11 @@
       <c r="E33">
         <v>4</v>
       </c>
-    </row>
-    <row r="34" spans="1:5">
+      <c r="F33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34" s="14">
         <v>0.627</v>
       </c>
@@ -2374,8 +2480,11 @@
       <c r="E34">
         <v>4</v>
       </c>
-    </row>
-    <row r="35" spans="1:5">
+      <c r="F34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35" s="16">
         <v>0.29699999999999999</v>
       </c>
@@ -2391,8 +2500,11 @@
       <c r="E35">
         <v>4</v>
       </c>
-    </row>
-    <row r="36" spans="1:5">
+      <c r="F35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
       <c r="A36" s="8">
         <v>0.504</v>
       </c>
@@ -2408,8 +2520,11 @@
       <c r="E36">
         <v>4</v>
       </c>
-    </row>
-    <row r="37" spans="1:5">
+      <c r="F36">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37" s="15">
         <v>0.40100000000000002</v>
       </c>
@@ -2425,8 +2540,11 @@
       <c r="E37">
         <v>4</v>
       </c>
-    </row>
-    <row r="38" spans="1:5">
+      <c r="F37">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
       <c r="A38" s="11">
         <v>0.17699999999999999</v>
       </c>
@@ -2442,8 +2560,11 @@
       <c r="E38">
         <v>4</v>
       </c>
-    </row>
-    <row r="39" spans="1:5">
+      <c r="F38">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
       <c r="A39" s="12">
         <v>9.6000000000000002E-2</v>
       </c>
@@ -2459,8 +2580,11 @@
       <c r="E39">
         <v>4</v>
       </c>
-    </row>
-    <row r="40" spans="1:5">
+      <c r="F39">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
       <c r="A40" s="16">
         <v>0.251</v>
       </c>
@@ -2476,8 +2600,11 @@
       <c r="E40">
         <v>4</v>
       </c>
-    </row>
-    <row r="41" spans="1:5">
+      <c r="F40">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
       <c r="A41" s="12">
         <v>7.0999999999999994E-2</v>
       </c>
@@ -2493,8 +2620,11 @@
       <c r="E41">
         <v>4</v>
       </c>
-    </row>
-    <row r="42" spans="1:5">
+      <c r="F41">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
       <c r="A42" s="10">
         <v>0.17699999999999999</v>
       </c>
@@ -2510,8 +2640,11 @@
       <c r="E42">
         <v>4</v>
       </c>
-    </row>
-    <row r="43" spans="1:5">
+      <c r="F42">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
       <c r="A43" s="16">
         <v>0.29699999999999999</v>
       </c>
@@ -2527,8 +2660,11 @@
       <c r="E43">
         <v>4</v>
       </c>
-    </row>
-    <row r="44" spans="1:5">
+      <c r="F43">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
       <c r="A44" s="16">
         <v>0.253</v>
       </c>
@@ -2544,8 +2680,11 @@
       <c r="E44">
         <v>4</v>
       </c>
-    </row>
-    <row r="45" spans="1:5">
+      <c r="F44">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
       <c r="A45" s="16">
         <v>0.25800000000000001</v>
       </c>
@@ -2561,8 +2700,11 @@
       <c r="E45">
         <v>4</v>
       </c>
-    </row>
-    <row r="46" spans="1:5">
+      <c r="F45">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
       <c r="A46" s="20">
         <v>0.56699999999999995</v>
       </c>
@@ -2578,8 +2720,11 @@
       <c r="E46">
         <v>4</v>
       </c>
-    </row>
-    <row r="47" spans="1:5">
+      <c r="F46">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
       <c r="A47" s="17">
         <v>0.69899999999999995</v>
       </c>
@@ -2595,8 +2740,11 @@
       <c r="E47">
         <v>4</v>
       </c>
-    </row>
-    <row r="48" spans="1:5">
+      <c r="F47">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
       <c r="A48" s="8">
         <v>0.50900000000000001</v>
       </c>
@@ -2612,8 +2760,11 @@
       <c r="E48">
         <v>4</v>
       </c>
-    </row>
-    <row r="49" spans="1:5">
+      <c r="F48">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
       <c r="A49" s="18">
         <v>0.83899999999999997</v>
       </c>
@@ -2629,8 +2780,11 @@
       <c r="E49">
         <v>4</v>
       </c>
-    </row>
-    <row r="50" spans="1:5">
+      <c r="F49">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
       <c r="A50" s="17">
         <v>0.68899999999999995</v>
       </c>
@@ -2646,8 +2800,11 @@
       <c r="E50">
         <v>4</v>
       </c>
-    </row>
-    <row r="51" spans="1:5">
+      <c r="F50">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
       <c r="A51" s="8">
         <v>0.50800000000000001</v>
       </c>
@@ -2663,8 +2820,11 @@
       <c r="E51">
         <v>4</v>
       </c>
-    </row>
-    <row r="52" spans="1:5">
+      <c r="F51">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
       <c r="A52" s="9">
         <v>0.33600000000000002</v>
       </c>
@@ -2680,8 +2840,11 @@
       <c r="E52">
         <v>4</v>
       </c>
-    </row>
-    <row r="53" spans="1:5">
+      <c r="F52">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
       <c r="A53" s="8">
         <v>0.496</v>
       </c>
@@ -2697,8 +2860,11 @@
       <c r="E53">
         <v>4</v>
       </c>
-    </row>
-    <row r="54" spans="1:5">
+      <c r="F53">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
       <c r="A54" s="19">
         <v>0.45400000000000001</v>
       </c>
@@ -2714,8 +2880,11 @@
       <c r="E54">
         <v>4</v>
       </c>
-    </row>
-    <row r="55" spans="1:5">
+      <c r="F54">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
       <c r="A55" s="19">
         <v>0.45500000000000002</v>
       </c>
@@ -2731,8 +2900,11 @@
       <c r="E55">
         <v>4</v>
       </c>
-    </row>
-    <row r="56" spans="1:5">
+      <c r="F55">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
       <c r="A56" s="17">
         <v>0.72299999999999998</v>
       </c>
@@ -2748,8 +2920,11 @@
       <c r="E56">
         <v>4</v>
       </c>
-    </row>
-    <row r="57" spans="1:5">
+      <c r="F56">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
       <c r="A57" s="14">
         <v>0.64</v>
       </c>
@@ -2765,8 +2940,11 @@
       <c r="E57">
         <v>4</v>
       </c>
-    </row>
-    <row r="58" spans="1:5">
+      <c r="F57">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
       <c r="A58" s="20">
         <v>0.56000000000000005</v>
       </c>
@@ -2782,8 +2960,11 @@
       <c r="E58">
         <v>4</v>
       </c>
-    </row>
-    <row r="59" spans="1:5">
+      <c r="F58">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
       <c r="A59" s="15">
         <v>0.39700000000000002</v>
       </c>
@@ -2799,8 +2980,11 @@
       <c r="E59">
         <v>4</v>
       </c>
-    </row>
-    <row r="60" spans="1:5">
+      <c r="F59">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
       <c r="A60" s="14">
         <v>0.628</v>
       </c>
@@ -2816,8 +3000,11 @@
       <c r="E60">
         <v>4</v>
       </c>
-    </row>
-    <row r="61" spans="1:5">
+      <c r="F60">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
       <c r="A61" s="15">
         <v>0.36799999999999999</v>
       </c>
@@ -2832,6 +3019,9 @@
       </c>
       <c r="E61">
         <v>4</v>
+      </c>
+      <c r="F61">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>